<commit_message>
fix: importThanhVienTrongHo fix key and null error
</commit_message>
<xml_diff>
--- a/App_Data/uploads/DIABAN.xlsx
+++ b/App_Data/uploads/DIABAN.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Haniki\SQL\tt1\import\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SQL\SQL practice\import\import\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E68DF88-13D4-4C42-B599-4E3A0C9C222D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30247371-3B0A-4991-B526-42DF1BFA1727}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{940A45BD-417B-4578-8F0E-AF31A061EAE4}"/>
+    <workbookView xWindow="3771" yWindow="1098" windowWidth="14918" windowHeight="9790" xr2:uid="{940A45BD-417B-4578-8F0E-AF31A061EAE4}"/>
   </bookViews>
   <sheets>
     <sheet name="DIABAN" sheetId="1" r:id="rId1"/>
@@ -179,9 +179,6 @@
     <t>Tổ dân phố 2 (Đầu ngách 2 ngõ 5, ngách 4, 6, 8, 10</t>
   </si>
   <si>
-    <t>Tổ dân phố 1</t>
-  </si>
-  <si>
     <t>TDP5-phường Trung Sơn Trầm</t>
   </si>
   <si>
@@ -191,9 +188,6 @@
     <t>Đông Lâu</t>
   </si>
   <si>
-    <t>Cụm 7-</t>
-  </si>
-  <si>
     <t>Xóm Hòa Lạc-</t>
   </si>
   <si>
@@ -519,6 +513,12 @@
   </si>
   <si>
     <t>X07092</t>
+  </si>
+  <si>
+    <t>Cụm 7</t>
+  </si>
+  <si>
+    <t>Tổ dân phố 1 (Phường Sơn Lộc)</t>
   </si>
 </sst>
 </file>
@@ -644,9 +644,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -684,7 +684,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -790,7 +790,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -932,7 +932,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -942,663 +942,663 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D577F55-C79C-4A61-8434-3BAE1F4A41EB}">
   <dimension ref="A1:B81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
-      <selection activeCell="C85" sqref="C84:C85"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="33.7109375" customWidth="1"/>
-    <col min="2" max="2" width="62.42578125" customWidth="1"/>
+    <col min="1" max="1" width="33.7265625" customWidth="1"/>
+    <col min="2" max="2" width="62.453125" customWidth="1"/>
     <col min="3" max="3" width="61" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="15.55" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15.55" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
         <v>80</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>82</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="15.55" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="15.55" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" ht="15.55" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" ht="15.55" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" ht="15.55" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" ht="15.55" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" ht="15.55" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" ht="15.55" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" ht="15.55" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" ht="15.55" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" ht="15.55" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" ht="15.55" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" ht="15.55" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" ht="15.55" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" ht="15.55" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" ht="15.55" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" ht="15.55" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" ht="15.55" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" ht="15.55" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" ht="15.55" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" ht="15.55" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" ht="15.55" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" ht="15.55" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" ht="15.55" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" ht="15.55" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" ht="15.55" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" ht="15.55" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" ht="15.55" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" ht="15.55" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" ht="15.55" x14ac:dyDescent="0.35">
       <c r="A32" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" ht="15.55" x14ac:dyDescent="0.35">
       <c r="A33" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" ht="15.55" x14ac:dyDescent="0.35">
       <c r="A34" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" ht="15.55" x14ac:dyDescent="0.35">
       <c r="A35" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" ht="15.55" x14ac:dyDescent="0.35">
       <c r="A36" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" ht="15.55" x14ac:dyDescent="0.35">
       <c r="A37" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" ht="15.55" x14ac:dyDescent="0.35">
       <c r="A38" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" ht="15.55" x14ac:dyDescent="0.35">
       <c r="A39" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" ht="15.55" x14ac:dyDescent="0.35">
       <c r="A40" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" ht="15.55" x14ac:dyDescent="0.35">
       <c r="A41" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" ht="15.55" x14ac:dyDescent="0.35">
       <c r="A42" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" ht="15.55" x14ac:dyDescent="0.35">
       <c r="A43" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" ht="15.55" x14ac:dyDescent="0.35">
       <c r="A44" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="45" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" ht="15.55" x14ac:dyDescent="0.35">
       <c r="A45" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="46" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" ht="15.55" x14ac:dyDescent="0.35">
       <c r="A46" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="47" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" ht="15.55" x14ac:dyDescent="0.35">
       <c r="A47" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B47" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="48" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" ht="15.55" x14ac:dyDescent="0.35">
       <c r="A48" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B48" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" ht="15.55" x14ac:dyDescent="0.35">
       <c r="A49" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B49" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="50" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" ht="15.55" x14ac:dyDescent="0.35">
       <c r="A50" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="15.55" x14ac:dyDescent="0.35">
+      <c r="A51" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="15.55" x14ac:dyDescent="0.35">
+      <c r="A52" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="B50" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A51" s="2" t="s">
+      <c r="B52" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="15.55" x14ac:dyDescent="0.35">
+      <c r="A53" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="B51" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A52" s="2" t="s">
+      <c r="B53" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" ht="15.55" x14ac:dyDescent="0.35">
+      <c r="A54" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="B52" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A53" s="2" t="s">
+      <c r="B54" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="15.55" x14ac:dyDescent="0.35">
+      <c r="A55" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="B53" s="2" t="s">
+      <c r="B55" s="2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="54" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A54" s="2" t="s">
+    <row r="56" spans="1:2" ht="15.55" x14ac:dyDescent="0.35">
+      <c r="A56" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="B54" s="2" t="s">
+      <c r="B56" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="55" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A55" s="2" t="s">
+    <row r="57" spans="1:2" ht="15.55" x14ac:dyDescent="0.35">
+      <c r="A57" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="B55" s="2" t="s">
+      <c r="B57" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="56" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A56" s="2" t="s">
+    <row r="58" spans="1:2" ht="15.55" x14ac:dyDescent="0.35">
+      <c r="A58" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="B56" s="2" t="s">
+      <c r="B58" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="57" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A57" s="2" t="s">
+    <row r="59" spans="1:2" ht="15.55" x14ac:dyDescent="0.35">
+      <c r="A59" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="B57" s="2" t="s">
+      <c r="B59" s="2" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="58" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A58" s="2" t="s">
+    <row r="60" spans="1:2" ht="15.55" x14ac:dyDescent="0.35">
+      <c r="A60" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="B58" s="2" t="s">
+      <c r="B60" s="2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="59" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A59" s="2" t="s">
+    <row r="61" spans="1:2" ht="15.55" x14ac:dyDescent="0.35">
+      <c r="A61" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="B59" s="2" t="s">
+      <c r="B61" s="2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="60" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A60" s="2" t="s">
+    <row r="62" spans="1:2" ht="15.55" x14ac:dyDescent="0.35">
+      <c r="A62" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="B60" s="2" t="s">
+      <c r="B62" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="61" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A61" s="2" t="s">
+    <row r="63" spans="1:2" ht="15.55" x14ac:dyDescent="0.35">
+      <c r="A63" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="B61" s="2" t="s">
+      <c r="B63" s="2" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="62" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A62" s="2" t="s">
+    <row r="64" spans="1:2" ht="15.55" x14ac:dyDescent="0.35">
+      <c r="A64" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="B62" s="2" t="s">
+      <c r="B64" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="63" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A63" s="2" t="s">
+    <row r="65" spans="1:2" ht="15.55" x14ac:dyDescent="0.35">
+      <c r="A65" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="B63" s="2" t="s">
+      <c r="B65" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="64" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A64" s="2" t="s">
+    <row r="66" spans="1:2" ht="15.55" x14ac:dyDescent="0.35">
+      <c r="A66" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="B64" s="2" t="s">
+      <c r="B66" s="2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="65" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A65" s="2" t="s">
+    <row r="67" spans="1:2" ht="15.55" x14ac:dyDescent="0.35">
+      <c r="A67" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="B65" s="2" t="s">
+      <c r="B67" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="66" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A66" s="2" t="s">
+    <row r="68" spans="1:2" ht="15.55" x14ac:dyDescent="0.35">
+      <c r="A68" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="B66" s="2" t="s">
+      <c r="B68" s="2" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="67" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A67" s="2" t="s">
+    <row r="69" spans="1:2" ht="15.55" x14ac:dyDescent="0.35">
+      <c r="A69" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="B67" s="2" t="s">
+      <c r="B69" s="2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="68" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A68" s="2" t="s">
+    <row r="70" spans="1:2" ht="15.55" x14ac:dyDescent="0.35">
+      <c r="A70" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="B68" s="2" t="s">
+      <c r="B70" s="2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="69" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A69" s="2" t="s">
+    <row r="71" spans="1:2" ht="15.55" x14ac:dyDescent="0.35">
+      <c r="A71" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="B69" s="2" t="s">
+      <c r="B71" s="2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="70" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A70" s="2" t="s">
+    <row r="72" spans="1:2" ht="15.55" x14ac:dyDescent="0.35">
+      <c r="A72" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="B70" s="2" t="s">
+      <c r="B72" s="2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="71" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A71" s="2" t="s">
+    <row r="73" spans="1:2" ht="15.55" x14ac:dyDescent="0.35">
+      <c r="A73" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="B71" s="2" t="s">
+      <c r="B73" s="2" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="72" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A72" s="2" t="s">
+    <row r="74" spans="1:2" ht="15.55" x14ac:dyDescent="0.35">
+      <c r="A74" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="B72" s="2" t="s">
+      <c r="B74" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="73" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A73" s="2" t="s">
+    <row r="75" spans="1:2" ht="15.55" x14ac:dyDescent="0.35">
+      <c r="A75" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="B73" s="2" t="s">
+      <c r="B75" s="2" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="74" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A74" s="2" t="s">
+    <row r="76" spans="1:2" ht="15.55" x14ac:dyDescent="0.35">
+      <c r="A76" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="B74" s="2" t="s">
+      <c r="B76" s="2" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="75" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A75" s="2" t="s">
+    <row r="77" spans="1:2" ht="15.55" x14ac:dyDescent="0.35">
+      <c r="A77" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="B75" s="2" t="s">
+      <c r="B77" s="2" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="76" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A76" s="2" t="s">
+    <row r="78" spans="1:2" ht="15.55" x14ac:dyDescent="0.35">
+      <c r="A78" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="B76" s="2" t="s">
+      <c r="B78" s="2" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="77" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A77" s="2" t="s">
+    <row r="79" spans="1:2" ht="15.55" x14ac:dyDescent="0.35">
+      <c r="A79" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="B77" s="2" t="s">
+      <c r="B79" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="78" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A78" s="2" t="s">
+    <row r="80" spans="1:2" ht="15.55" x14ac:dyDescent="0.35">
+      <c r="A80" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="B78" s="2" t="s">
+      <c r="B80" s="2" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="79" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A79" s="2" t="s">
+    <row r="81" spans="1:2" ht="15.55" x14ac:dyDescent="0.35">
+      <c r="A81" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="B79" s="2" t="s">
+      <c r="B81" s="2" t="s">
         <v>77</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A80" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="B80" s="2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A81" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="B81" s="2" t="s">
-        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>